<commit_message>
first two output tables generated
</commit_message>
<xml_diff>
--- a/Outputs.xlsx
+++ b/Outputs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F29E69-8197-4B0B-8748-700CA743B47F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="forecastSMI_allPeriods" sheetId="1" r:id="rId1"/>
@@ -12,17 +13,22 @@
     <sheet name="intSMI_FX1.20" sheetId="3" r:id="rId3"/>
     <sheet name="intSMI_SD75quantile" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="469">
   <si>
     <t>&gt; forecastSMI</t>
   </si>
@@ -711,240 +717,84 @@
     <t>$IntTrainError</t>
   </si>
   <si>
-    <t>[1] 35.40494</t>
-  </si>
-  <si>
     <t>$IntTestError</t>
   </si>
   <si>
-    <t>[1] 43.1448</t>
-  </si>
-  <si>
     <t>$IntTestPValue.p.value</t>
   </si>
   <si>
-    <t>[1] 1.727403e-190</t>
-  </si>
-  <si>
     <t>$IntVarImp.SDdomBanksdir</t>
   </si>
   <si>
-    <t>[1] 87.15804</t>
-  </si>
-  <si>
     <t>$IntVarImp.SMIprev</t>
   </si>
   <si>
-    <t>[1] 54.26782</t>
-  </si>
-  <si>
     <t>$IntVarImp.Libor3M_CHF</t>
   </si>
   <si>
-    <t>[1] 23.79887</t>
-  </si>
-  <si>
     <t>$IntVarImp.SDofDomBanks</t>
   </si>
   <si>
-    <t>[1] 6.528867</t>
-  </si>
-  <si>
     <t>$IntVarImp.CHFUSD</t>
   </si>
   <si>
-    <t>[1] 5.588393</t>
-  </si>
-  <si>
     <t>$IntVarImp.CHFEUR</t>
   </si>
   <si>
-    <t>[1] 5.178465</t>
-  </si>
-  <si>
     <t>$IntVarImp.ChgSDdomBanks</t>
   </si>
   <si>
-    <t>[1] 3.761699</t>
-  </si>
-  <si>
     <t>$IntVarImp.Gov3yr</t>
   </si>
   <si>
-    <t>[1] 2.994696</t>
-  </si>
-  <si>
     <t>$IntVarImp.Gov10yr</t>
   </si>
   <si>
-    <t>[1] 2.774562</t>
-  </si>
-  <si>
     <t>$NoIntTrainError</t>
   </si>
   <si>
-    <t>[1] 40.16565</t>
-  </si>
-  <si>
     <t>$NoIntTestError</t>
   </si>
   <si>
-    <t>[1] 49.20109</t>
-  </si>
-  <si>
     <t>$NoIntTestPValue.p.value</t>
   </si>
   <si>
-    <t>[1] 2.159934e-05</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.SDdomBanksdir</t>
   </si>
   <si>
-    <t>[1] 38.51826</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.CHFUSD</t>
   </si>
   <si>
-    <t>[1] 19.82078</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.Libor3M_CHF</t>
   </si>
   <si>
-    <t>[1] 17.43124</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.ChgSDdomBanks</t>
   </si>
   <si>
-    <t>[1] 13.64863</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.Gov3yr</t>
   </si>
   <si>
-    <t>[1] 13.3062</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.SDofDomBanks</t>
   </si>
   <si>
-    <t>[1] 11.6078</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.Gov10yr</t>
   </si>
   <si>
-    <t>[1] 3.9485</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.SMIprev</t>
   </si>
   <si>
-    <t>[1] 2.469348</t>
-  </si>
-  <si>
     <t>$NoIntVarImp.CHFEUR</t>
   </si>
   <si>
-    <t>[1] 1.433913</t>
-  </si>
-  <si>
     <t>$WelchSDDirPValue</t>
   </si>
   <si>
-    <t>[1] 7.081045e-84</t>
-  </si>
-  <si>
     <t>$WelchSDPValue</t>
   </si>
   <si>
-    <t>[1] 0.0008876137</t>
-  </si>
-  <si>
     <t>[1] "interventionC5"</t>
   </si>
   <si>
-    <t>[1] 35.40776</t>
-  </si>
-  <si>
-    <t>[1] 43.306</t>
-  </si>
-  <si>
-    <t>[1] 5.923989e-173</t>
-  </si>
-  <si>
-    <t>[1] 51.79706</t>
-  </si>
-  <si>
-    <t>[1] 31.61576</t>
-  </si>
-  <si>
-    <t>[1] 7.902903</t>
-  </si>
-  <si>
-    <t>[1] 2.332086</t>
-  </si>
-  <si>
-    <t>[1] 1.676012</t>
-  </si>
-  <si>
-    <t>[1] 1.470962</t>
-  </si>
-  <si>
-    <t>[1] 1.20959</t>
-  </si>
-  <si>
-    <t>[1] 1.098457</t>
-  </si>
-  <si>
-    <t>[1] 0.897174</t>
-  </si>
-  <si>
-    <t>[1] 40.30815</t>
-  </si>
-  <si>
-    <t>[1] 49.24501</t>
-  </si>
-  <si>
-    <t>[1] 3.006029e-05</t>
-  </si>
-  <si>
-    <t>[1] 36.77229</t>
-  </si>
-  <si>
-    <t>[1] 15.87223</t>
-  </si>
-  <si>
-    <t>[1] 14.847</t>
-  </si>
-  <si>
-    <t>[1] 10.3329</t>
-  </si>
-  <si>
-    <t>[1] 7.00036</t>
-  </si>
-  <si>
-    <t>[1] 6.694187</t>
-  </si>
-  <si>
-    <t>[1] 3.032485</t>
-  </si>
-  <si>
-    <t>[1] 2.892386</t>
-  </si>
-  <si>
-    <t>[1] 2.556158</t>
-  </si>
-  <si>
-    <t>[1] 6.260934e-16</t>
-  </si>
-  <si>
-    <t>[1] 1.010448e-07</t>
-  </si>
-  <si>
     <t>&gt; InterventionCurrentSMI_Sd75</t>
   </si>
   <si>
@@ -1020,82 +870,577 @@
     <t>[1] 6.045897e-47</t>
   </si>
   <si>
-    <t>[1] 32.95616</t>
-  </si>
-  <si>
-    <t>[1] 42.47919</t>
-  </si>
-  <si>
-    <t>[1] 4.553248e-148</t>
-  </si>
-  <si>
-    <t>[1] 91.51399</t>
-  </si>
-  <si>
-    <t>[1] 22.04218</t>
-  </si>
-  <si>
-    <t>[1] 20.49321</t>
-  </si>
-  <si>
-    <t>[1] 9.361071</t>
-  </si>
-  <si>
-    <t>[1] 7.042204</t>
-  </si>
-  <si>
-    <t>[1] 5.975813</t>
-  </si>
-  <si>
-    <t>[1] 5.021897</t>
-  </si>
-  <si>
-    <t>[1] 4.128608</t>
-  </si>
-  <si>
-    <t>[1] 43.27179</t>
-  </si>
-  <si>
-    <t>[1] 50.23026</t>
-  </si>
-  <si>
-    <t>[1] 0.1294698</t>
-  </si>
-  <si>
-    <t>[1] 65.99874</t>
-  </si>
-  <si>
-    <t>[1] 14.34856</t>
-  </si>
-  <si>
-    <t>[1] 11.31992</t>
-  </si>
-  <si>
-    <t>[1] 7.246692</t>
-  </si>
-  <si>
-    <t>[1] 5.647949</t>
-  </si>
-  <si>
-    <t>[1] 2.558897</t>
-  </si>
-  <si>
-    <t>[1] 2.517667</t>
-  </si>
-  <si>
-    <t>[1] 1.796641</t>
-  </si>
-  <si>
-    <t>[1] 3.270768e-24</t>
-  </si>
-  <si>
-    <t>[1] 1.473193e-38</t>
+    <t>\begin{table}[ht]</t>
+  </si>
+  <si>
+    <t>\centering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  \hline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  \hline\hline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   \hline</t>
+  </si>
+  <si>
+    <t>\end{tabular}</t>
+  </si>
+  <si>
+    <t>\end{table}</t>
+  </si>
+  <si>
+    <t>SDdomBanksdir</t>
+  </si>
+  <si>
+    <t>SDofDomBanks</t>
+  </si>
+  <si>
+    <t>SMIprev</t>
+  </si>
+  <si>
+    <t>Gov3yr</t>
+  </si>
+  <si>
+    <t>CHFUSD</t>
+  </si>
+  <si>
+    <t>Gov10yr</t>
+  </si>
+  <si>
+    <t>Libor3M_CHF</t>
+  </si>
+  <si>
+    <t>CHFEUR</t>
+  </si>
+  <si>
+    <t>$`IntTrainError`</t>
+  </si>
+  <si>
+    <t>[1] 35.39074</t>
+  </si>
+  <si>
+    <t>[1] 42.90113</t>
+  </si>
+  <si>
+    <t>[1] 3.236177e-193</t>
+  </si>
+  <si>
+    <t>[1] 89.44803</t>
+  </si>
+  <si>
+    <t>[1] 55.66236</t>
+  </si>
+  <si>
+    <t>[1] 23.87921</t>
+  </si>
+  <si>
+    <t>[1] 6.078745</t>
+  </si>
+  <si>
+    <t>[1] 5.632037</t>
+  </si>
+  <si>
+    <t>[1] 5.236142</t>
+  </si>
+  <si>
+    <t>[1] 3.157469</t>
+  </si>
+  <si>
+    <t>[1] 2.681687</t>
+  </si>
+  <si>
+    <t>[1] 2.25321</t>
+  </si>
+  <si>
+    <t>[1] 40.17484</t>
+  </si>
+  <si>
+    <t>[1] 49.12939</t>
+  </si>
+  <si>
+    <t>[1] 3.198019e-07</t>
+  </si>
+  <si>
+    <t>[1] 39.35717</t>
+  </si>
+  <si>
+    <t>[1] 19.39683</t>
+  </si>
+  <si>
+    <t>[1] 16.86922</t>
+  </si>
+  <si>
+    <t>[1] 16.10055</t>
+  </si>
+  <si>
+    <t>[1] 12.8903</t>
+  </si>
+  <si>
+    <t>[1] 10.38277</t>
+  </si>
+  <si>
+    <t>[1] 5.382875</t>
+  </si>
+  <si>
+    <t>[1] 4.231797</t>
+  </si>
+  <si>
+    <t>[1] 2.12797</t>
+  </si>
+  <si>
+    <t>[1] 6.917382e-92</t>
+  </si>
+  <si>
+    <t>[1] 1.973022e-05</t>
+  </si>
+  <si>
+    <t>[1] 35.50133</t>
+  </si>
+  <si>
+    <t>[1] 43.15216</t>
+  </si>
+  <si>
+    <t>[1] 1.87623e-190</t>
+  </si>
+  <si>
+    <t>[1] 52.77046</t>
+  </si>
+  <si>
+    <t>[1] 30.74901</t>
+  </si>
+  <si>
+    <t>[1] 8.238496</t>
+  </si>
+  <si>
+    <t>[1] 2.048559</t>
+  </si>
+  <si>
+    <t>[1] 1.620808</t>
+  </si>
+  <si>
+    <t>[1] 1.521323</t>
+  </si>
+  <si>
+    <t>[1] 1.172037</t>
+  </si>
+  <si>
+    <t>[1] 1.01204</t>
+  </si>
+  <si>
+    <t>[1] 0.8672684</t>
+  </si>
+  <si>
+    <t>[1] 40.20534</t>
+  </si>
+  <si>
+    <t>[1] 49.48462</t>
+  </si>
+  <si>
+    <t>[1] 0.003403553</t>
+  </si>
+  <si>
+    <t>[1] 37.58186</t>
+  </si>
+  <si>
+    <t>[1] 13.57149</t>
+  </si>
+  <si>
+    <t>[1] 11.70081</t>
+  </si>
+  <si>
+    <t>[1] 11.65583</t>
+  </si>
+  <si>
+    <t>[1] 8.523074</t>
+  </si>
+  <si>
+    <t>[1] 8.157783</t>
+  </si>
+  <si>
+    <t>[1] 3.529263</t>
+  </si>
+  <si>
+    <t>[1] 2.656001</t>
+  </si>
+  <si>
+    <t>[1] 2.623894</t>
+  </si>
+  <si>
+    <t>[1] 7.229343e-16</t>
+  </si>
+  <si>
+    <t>[1] 3.467045e-08</t>
+  </si>
+  <si>
+    <t>ChgSDdomBanks</t>
+  </si>
+  <si>
+    <t>[1] 32.72584</t>
+  </si>
+  <si>
+    <t>[1] 43.1131</t>
+  </si>
+  <si>
+    <t>[1] 4.16283e-140</t>
+  </si>
+  <si>
+    <t>[1] 87.32558</t>
+  </si>
+  <si>
+    <t>[1] 24.87181</t>
+  </si>
+  <si>
+    <t>[1] 17.03225</t>
+  </si>
+  <si>
+    <t>[1] 9.900901</t>
+  </si>
+  <si>
+    <t>[1] 6.346959</t>
+  </si>
+  <si>
+    <t>[1] 5.725601</t>
+  </si>
+  <si>
+    <t>[1] 3.853413</t>
+  </si>
+  <si>
+    <t>[1] 3.427248</t>
+  </si>
+  <si>
+    <t>[1] 43.46392</t>
+  </si>
+  <si>
+    <t>[1] 50.29201</t>
+  </si>
+  <si>
+    <t>[1] 0.06780446</t>
+  </si>
+  <si>
+    <t>[1] 69.27781</t>
+  </si>
+  <si>
+    <t>[1] 12.2976</t>
+  </si>
+  <si>
+    <t>[1] 10.77802</t>
+  </si>
+  <si>
+    <t>[1] 7.553067</t>
+  </si>
+  <si>
+    <t>[1] 6.072268</t>
+  </si>
+  <si>
+    <t>[1] 2.979459</t>
+  </si>
+  <si>
+    <t>[1] 1.752242</t>
+  </si>
+  <si>
+    <t>[1] 1.442577</t>
+  </si>
+  <si>
+    <t>[1] 1.078478e-13</t>
+  </si>
+  <si>
+    <t>[1] 2.984368e-55</t>
+  </si>
+  <si>
+    <t>52.77</t>
+  </si>
+  <si>
+    <t>89.45</t>
+  </si>
+  <si>
+    <t>30.75</t>
+  </si>
+  <si>
+    <t>55.66</t>
+  </si>
+  <si>
+    <t>8.24</t>
+  </si>
+  <si>
+    <t>23.88</t>
+  </si>
+  <si>
+    <t>2.05</t>
+  </si>
+  <si>
+    <t>6.08</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>3.16</t>
+  </si>
+  <si>
+    <t>1.52</t>
+  </si>
+  <si>
+    <t>5.63</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>5.24</t>
+  </si>
+  <si>
+    <t>1.01</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>2.68</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>noint</t>
+  </si>
+  <si>
+    <t>37.58</t>
+  </si>
+  <si>
+    <t>39.36</t>
+  </si>
+  <si>
+    <t>13.57</t>
+  </si>
+  <si>
+    <t>16.87</t>
+  </si>
+  <si>
+    <t>11.70</t>
+  </si>
+  <si>
+    <t>19.40</t>
+  </si>
+  <si>
+    <t>11.66</t>
+  </si>
+  <si>
+    <t>16.10</t>
+  </si>
+  <si>
+    <t>8.52</t>
+  </si>
+  <si>
+    <t>10.38</t>
+  </si>
+  <si>
+    <t>8.16</t>
+  </si>
+  <si>
+    <t>12.89</t>
+  </si>
+  <si>
+    <t>3.53</t>
+  </si>
+  <si>
+    <t>5.38</t>
+  </si>
+  <si>
+    <t>2.66</t>
+  </si>
+  <si>
+    <t>2.13</t>
+  </si>
+  <si>
+    <t>2.62</t>
+  </si>
+  <si>
+    <t>4.23</t>
+  </si>
+  <si>
+    <t>\caption{C5.0 output for the FX Intervention Set (CHF/EUR &lt; 1.20). Train Error 35.5\% / 40.2\%. Test Error 43.05\%*** / 49.3\%**. }</t>
+  </si>
+  <si>
+    <t>\label{Output IntFX}</t>
+  </si>
+  <si>
+    <t>\begin{tabular}{||c c c c c||}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Variable importance &amp; Splits (Int) &amp; Usage (Int) &amp; Splits (NoInt) &amp; Usage (NoInt)\\ [0.5ex] </t>
+  </si>
+  <si>
+    <t>10.37</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>20.49</t>
+  </si>
+  <si>
+    <t>4.13</t>
+  </si>
+  <si>
+    <t>9.36</t>
+  </si>
+  <si>
+    <t>3.77</t>
+  </si>
+  <si>
+    <t>5.98</t>
+  </si>
+  <si>
+    <t>2.46</t>
+  </si>
+  <si>
+    <t>7.04</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>5.02</t>
+  </si>
+  <si>
+    <t>1.90</t>
+  </si>
+  <si>
+    <t>62.15</t>
+  </si>
+  <si>
+    <t>66.00</t>
+  </si>
+  <si>
+    <t>11.42</t>
+  </si>
+  <si>
+    <t>11.32</t>
+  </si>
+  <si>
+    <t>7.58</t>
+  </si>
+  <si>
+    <t>14.35</t>
+  </si>
+  <si>
+    <t>6.79</t>
+  </si>
+  <si>
+    <t>5.65</t>
+  </si>
+  <si>
+    <t>5.57</t>
+  </si>
+  <si>
+    <t>2.56</t>
+  </si>
+  <si>
+    <t>4.74</t>
+  </si>
+  <si>
+    <t>7.25</t>
+  </si>
+  <si>
+    <t>1.44</t>
+  </si>
+  <si>
+    <t>1.80</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>2.52</t>
+  </si>
+  <si>
+    <t>[1] 32.48123</t>
+  </si>
+  <si>
+    <t>[1] 42.71102</t>
+  </si>
+  <si>
+    <t>[1] 6.536198e-303</t>
+  </si>
+  <si>
+    <t>[1] 66.06749</t>
+  </si>
+  <si>
+    <t>[1] 10.7686</t>
+  </si>
+  <si>
+    <t>[1] 8.538899</t>
+  </si>
+  <si>
+    <t>[1] 4.195184</t>
+  </si>
+  <si>
+    <t>[1] 4.184096</t>
+  </si>
+  <si>
+    <t>[1] 2.136453</t>
+  </si>
+  <si>
+    <t>[1] 2.136097</t>
+  </si>
+  <si>
+    <t>[1] 1.973179</t>
+  </si>
+  <si>
+    <t>[1] 43.36722</t>
+  </si>
+  <si>
+    <t>[1] 50.28709</t>
+  </si>
+  <si>
+    <t>[1] 0.009477735</t>
+  </si>
+  <si>
+    <t>[1] 60.44622</t>
+  </si>
+  <si>
+    <t>[1] 11.12832</t>
+  </si>
+  <si>
+    <t>[1] 9.082097</t>
+  </si>
+  <si>
+    <t>[1] 7.577161</t>
+  </si>
+  <si>
+    <t>[1] 4.892213</t>
+  </si>
+  <si>
+    <t>[1] 4.077971</t>
+  </si>
+  <si>
+    <t>[1] 1.594649</t>
+  </si>
+  <si>
+    <t>[1] 1.201367</t>
+  </si>
+  <si>
+    <t>[1] 0.0007883038</t>
+  </si>
+  <si>
+    <t>[1] 2.142242e-71</t>
+  </si>
+  <si>
+    <t>\caption{C5.0 output for the large SD Changes Intervention Set (75% Quantile of absolute Changes). Train Error 32.5\% / 43.4\%. Test Error 42.9\%*** / 50.3\%**. }</t>
+  </si>
+  <si>
+    <t>\label{Output IntSD}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1125,7 +1470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1135,6 +1480,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1151,7 +1502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1166,6 +1517,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1445,7 +1800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C534"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3720,7 +4075,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5127,20 +5482,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="4" width="35.42578125" customWidth="1"/>
+    <col min="1" max="2" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>179</v>
       </c>
@@ -5148,7 +5504,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>227</v>
       </c>
@@ -5156,523 +5512,829 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>228</v>
+        <v>295</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>282</v>
+        <v>323</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>285</v>
+        <v>326</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="I16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="I17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="I18" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>286</v>
+        <v>327</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="I19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G20" t="s">
+        <v>392</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="I20" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="E21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I21" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>373</v>
+      </c>
+      <c r="F22" t="s">
+        <v>374</v>
+      </c>
+      <c r="G22" t="s">
+        <v>393</v>
+      </c>
+      <c r="H22" t="s">
+        <v>394</v>
+      </c>
+      <c r="I22" s="7" t="str">
+        <f>D22&amp;" &amp; "&amp;E22&amp;" &amp; "&amp;F22&amp;" &amp; "&amp;G22&amp;" &amp; "&amp;H22&amp;" \\"</f>
+        <v>SDdomBanksdir &amp; 52.77 &amp; 89.45 &amp; 37.58 &amp; 39.36 \\</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E23" t="s">
+        <v>375</v>
+      </c>
+      <c r="F23" t="s">
+        <v>376</v>
+      </c>
+      <c r="G23" t="s">
+        <v>409</v>
+      </c>
+      <c r="H23" t="s">
+        <v>410</v>
+      </c>
+      <c r="I23" s="7" t="str">
+        <f t="shared" ref="I23:I30" si="0">D23&amp;" &amp; "&amp;E23&amp;" &amp; "&amp;F23&amp;" &amp; "&amp;G23&amp;" &amp; "&amp;H23&amp;" \\"</f>
+        <v>SMIprev &amp; 30.75 &amp; 55.66 &amp; 2.62 &amp; 4.23 \\</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" t="s">
+        <v>377</v>
+      </c>
+      <c r="F24" t="s">
+        <v>378</v>
+      </c>
+      <c r="G24" t="s">
+        <v>399</v>
+      </c>
+      <c r="H24" t="s">
+        <v>400</v>
+      </c>
+      <c r="I24" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Libor3M_CHF &amp; 8.24 &amp; 23.88 &amp; 11.66 &amp; 16.10 \\</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>379</v>
+      </c>
+      <c r="F25" t="s">
+        <v>380</v>
+      </c>
+      <c r="G25" t="s">
+        <v>403</v>
+      </c>
+      <c r="H25" t="s">
+        <v>404</v>
+      </c>
+      <c r="I25" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>SDofDomBanks &amp; 2.05 &amp; 6.08 &amp; 8.16 &amp; 12.89 \\</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F26" t="s">
+        <v>382</v>
+      </c>
+      <c r="G26" t="s">
+        <v>401</v>
+      </c>
+      <c r="H26" t="s">
+        <v>402</v>
+      </c>
+      <c r="I26" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>ChgSDdomBanks &amp; 1.62 &amp; 3.16 &amp; 8.52 &amp; 10.38 \\</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E27" t="s">
+        <v>383</v>
+      </c>
+      <c r="F27" t="s">
+        <v>384</v>
+      </c>
+      <c r="G27" t="s">
+        <v>407</v>
+      </c>
+      <c r="H27" t="s">
+        <v>408</v>
+      </c>
+      <c r="I27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>CHFEUR &amp; 1.52 &amp; 5.63 &amp; 2.66 &amp; 2.13 \\</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>289</v>
+        <v>330</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E28" t="s">
+        <v>385</v>
+      </c>
+      <c r="F28" t="s">
+        <v>386</v>
+      </c>
+      <c r="G28" t="s">
+        <v>397</v>
+      </c>
+      <c r="H28" t="s">
+        <v>398</v>
+      </c>
+      <c r="I28" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>CHFUSD &amp; 1.17 &amp; 5.24 &amp; 11.70 &amp; 19.40 \\</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E29" t="s">
+        <v>387</v>
+      </c>
+      <c r="F29" t="s">
+        <v>388</v>
+      </c>
+      <c r="G29" t="s">
+        <v>405</v>
+      </c>
+      <c r="H29" t="s">
+        <v>406</v>
+      </c>
+      <c r="I29" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Gov10yr &amp; 1.01 &amp; 2.25 &amp; 3.53 &amp; 5.38 \\</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E30" t="s">
+        <v>389</v>
+      </c>
+      <c r="F30" t="s">
+        <v>390</v>
+      </c>
+      <c r="G30" t="s">
+        <v>395</v>
+      </c>
+      <c r="H30" t="s">
+        <v>396</v>
+      </c>
+      <c r="I30" s="7" t="str">
+        <f>D30&amp;" &amp; "&amp;E30&amp;" &amp; "&amp;F30&amp;" &amp; "&amp;G30&amp;" &amp; "&amp;H30&amp;" \\ [1ex]"</f>
+        <v>Gov3yr &amp; 0.87 &amp; 2.68 &amp; 13.57 &amp; 16.87 \\ [1ex]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>290</v>
+        <v>331</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+      <c r="I31" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="I32" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="I33" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>291</v>
+        <v>332</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="I34" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="I35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>292</v>
+        <v>333</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>293</v>
+        <v>334</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>294</v>
+        <v>335</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>295</v>
+        <v>336</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>296</v>
+        <v>337</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>297</v>
+        <v>338</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>298</v>
+        <v>339</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>299</v>
+        <v>340</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>300</v>
+        <v>341</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>301</v>
+        <v>342</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>302</v>
+        <v>343</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D68" s="1"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>303</v>
+        <v>344</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="D72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>305</v>
+        <v>346</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>
@@ -5686,544 +6348,982 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="D33:F41">
+    <sortCondition descending="1" ref="E33:E41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>307</v>
+        <v>255</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>228</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>308</v>
+        <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>309</v>
+        <v>257</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="J7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="J8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="J9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>310</v>
+        <v>258</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="J10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="J11" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="J12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E13" t="s">
+        <v>287</v>
+      </c>
+      <c r="F13">
+        <v>66.06</v>
+      </c>
+      <c r="G13">
+        <v>87.33</v>
+      </c>
+      <c r="H13" t="s">
+        <v>427</v>
+      </c>
+      <c r="I13" t="s">
+        <v>428</v>
+      </c>
+      <c r="J13" s="7" t="str">
+        <f t="shared" ref="J13:J19" si="0">E13&amp;" &amp; "&amp;F13&amp;" &amp; "&amp;G13&amp;" &amp; "&amp;H13&amp;" &amp; "&amp;I13&amp;" \\"</f>
+        <v>SDdomBanksdir &amp; 66.06 &amp; 87.33 &amp; 62.15 &amp; 66.00 \\</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="E14" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" t="s">
+        <v>415</v>
+      </c>
+      <c r="G14">
+        <v>24.87</v>
+      </c>
+      <c r="H14" t="s">
+        <v>441</v>
+      </c>
+      <c r="I14" t="s">
+        <v>442</v>
+      </c>
+      <c r="J14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>SDofDomBanks &amp; 10.37 &amp; 24.87 &amp; 0.31 &amp; 2.52 \\</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E15" t="s">
+        <v>289</v>
+      </c>
+      <c r="F15" t="s">
+        <v>416</v>
+      </c>
+      <c r="G15" t="s">
+        <v>417</v>
+      </c>
+      <c r="H15" t="s">
+        <v>431</v>
+      </c>
+      <c r="I15" t="s">
+        <v>432</v>
+      </c>
+      <c r="J15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>SMIprev &amp; 8.00 &amp; 20.49 &amp; 7.58 &amp; 14.35 \\</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>312</v>
+        <v>260</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E16" t="s">
+        <v>290</v>
+      </c>
+      <c r="F16" t="s">
+        <v>418</v>
+      </c>
+      <c r="G16" t="s">
+        <v>419</v>
+      </c>
+      <c r="H16" t="s">
+        <v>433</v>
+      </c>
+      <c r="I16" t="s">
+        <v>434</v>
+      </c>
+      <c r="J16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Gov3yr &amp; 4.13 &amp; 9.36 &amp; 6.79 &amp; 5.65 \\</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="E17" t="s">
+        <v>291</v>
+      </c>
+      <c r="F17" t="s">
+        <v>420</v>
+      </c>
+      <c r="G17" t="s">
+        <v>421</v>
+      </c>
+      <c r="H17" t="s">
+        <v>437</v>
+      </c>
+      <c r="I17" t="s">
+        <v>438</v>
+      </c>
+      <c r="J17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>CHFUSD &amp; 3.77 &amp; 5.98 &amp; 4.74 &amp; 7.25 \\</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E18" t="s">
+        <v>292</v>
+      </c>
+      <c r="F18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G18" t="s">
+        <v>423</v>
+      </c>
+      <c r="H18" t="s">
+        <v>439</v>
+      </c>
+      <c r="I18" t="s">
+        <v>440</v>
+      </c>
+      <c r="J18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Gov10yr &amp; 2.46 &amp; 7.04 &amp; 1.44 &amp; 1.80 \\</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>313</v>
+        <v>261</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F19" t="s">
+        <v>424</v>
+      </c>
+      <c r="G19" t="s">
+        <v>425</v>
+      </c>
+      <c r="H19" t="s">
+        <v>429</v>
+      </c>
+      <c r="I19" t="s">
+        <v>430</v>
+      </c>
+      <c r="J19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Libor3M_CHF &amp; 2.10 &amp; 5.02 &amp; 11.42 &amp; 11.32 \\</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="E20" t="s">
+        <v>294</v>
+      </c>
+      <c r="F20" t="s">
+        <v>426</v>
+      </c>
+      <c r="G20" t="s">
+        <v>418</v>
+      </c>
+      <c r="H20" t="s">
+        <v>435</v>
+      </c>
+      <c r="I20" t="s">
+        <v>436</v>
+      </c>
+      <c r="J20" s="7" t="str">
+        <f>E20&amp;" &amp; "&amp;F20&amp;" &amp; "&amp;G20&amp;" &amp; "&amp;H20&amp;" &amp; "&amp;I20&amp;" \\ [1ex]"</f>
+        <v>CHFEUR &amp; 1.90 &amp; 4.13 &amp; 5.57 &amp; 2.56 \\ [1ex]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="J21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>314</v>
+        <v>262</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="J22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="E23" s="3"/>
+      <c r="J23" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="J24" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>315</v>
+        <v>263</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="J25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>316</v>
+        <v>264</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>317</v>
+        <v>265</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>318</v>
+        <v>266</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>319</v>
+        <v>267</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>320</v>
+        <v>268</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>321</v>
+        <v>269</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>322</v>
+        <v>270</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>323</v>
+        <v>271</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="B52" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>325</v>
+        <v>273</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="B58" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>327</v>
+        <v>275</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>328</v>
+        <v>276</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>329</v>
+        <v>277</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>330</v>
+        <v>278</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>331</v>
+        <v>279</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>280</v>
+        <v>254</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="E29:G36">
+    <sortCondition descending="1" ref="F29:F36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>